<commit_message>
Update CYRS review sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -155,9 +155,6 @@
     <t xml:space="preserve">You need to make your requirement more clarified from the system level prospective. 
 In REQ_PO2EBL_CYRS_02_V02 instead of saying when the switch is pressed again, the blender shall operate on the higher speed level until it reaches the maximum level, and the next press shall turn it off.
 You can say: the blender shall operate between 3 different speeds (Speed1 → Speed 2 → Speed 3) triggered by a button press after the fourth press it returns back to its initial state (off).  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
   </si>
   <si>
     <t xml:space="preserve">AAL 7/2/2020 : This point will be still open until remove from Imp#HW as we discussed that any requirements related to HW must be described and clarified well from HW prospective inside HSI document. </t>
@@ -194,6 +191,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
     <t xml:space="preserve">REQ_PO2EBL_CYRS_04_V02: 
 There isn’t a customer specification states that you need to turn on a corresponding led according to changing in speed levels. You shouldn’t take a step forward and guess something not mentioned by the customer in CRS until taking customer approval. 
 </t>
@@ -202,7 +202,10 @@
     <t xml:space="preserve">V1.8</t>
   </si>
   <si>
-    <t xml:space="preserve">Version Date is different from the Date field in Release Table in page 2 , plaese apply a unique Date format for all date fields, add a title before the table in second page.</t>
+    <t xml:space="preserve">Version Date is different from the Date field in Release Table in page 2 , please apply a unique Date format for all date fields, add a title before the table in second page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAL 10/2/2020 : there’s no title added before the table in second page. </t>
   </si>
   <si>
     <t xml:space="preserve">Page 6</t>
@@ -211,6 +214,27 @@
     <t xml:space="preserve">As discussed before Hardware Section shall be written in HSI document and instead of this section you can add a block diagram which describe how the system components interact with each others (I/Ps &amp; O/Ps).</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AAL 10/2/2020: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">add a block diagram which describe how the system components interact with each others (I/Ps &amp; O/Ps).</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Page 3</t>
   </si>
   <si>
@@ -221,6 +245,16 @@
   </si>
   <si>
     <t xml:space="preserve">whether to accept the open point if you see applicable and valid or to refuse it and give a justification in the comment field whether you accept , then update with the action you did , or refuse with justification </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You need to add more requirements in CYRS which illustrate some features in your system 
+Ex: you can  add requirements which describe how to handle the communication between the inputs devices &amp; o/p devices.</t>
   </si>
   <si>
     <t xml:space="preserve">Status </t>
@@ -241,7 +275,7 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="[$-409]MM/DD/YY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -294,6 +328,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -323,7 +363,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -597,7 +637,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,7 +645,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -625,11 +665,23 @@
     <cellStyle name="Normal 4" xfId="21"/>
     <cellStyle name="Excel Built-in Accent3" xfId="22"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFC00000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -642,15 +694,15 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFDAE3F3"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -660,29 +712,29 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFBE5D6"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFA5A5A5"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF70AD47"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF535353"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF1F4E79"/>
-      <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -699,7 +751,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.27"/>
   </cols>
@@ -940,12 +992,12 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.54"/>
@@ -1122,10 +1174,10 @@
         <v>32</v>
       </c>
       <c r="H6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="22" t="s">
         <v>43</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="52.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1145,17 +1197,17 @@
         <v>38</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I7" s="22"/>
       <c r="K7" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="57.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1233,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I8" s="20"/>
       <c r="K8" s="0" t="s">
@@ -1209,11 +1261,13 @@
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="20"/>
-    </row>
-    <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="n">
         <v>44014</v>
       </c>
@@ -1227,16 +1281,18 @@
         <v>3</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="20"/>
+        <v>45</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="n">
@@ -1252,38 +1308,52 @@
         <v>29</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I11" s="20"/>
       <c r="K11" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="24" t="n">
+        <v>44106</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="H12" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="I12" s="20"/>
       <c r="K12" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update the CYRS,update the date format Add Block diagram and Add  Control inputs with outputs REQ_PO2EBL_CYRS_04_V1.0 Signed-off-by: Mohammmedibra96 <mohammedibra96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS/CYRS_Review.xlsx
+++ b/Input documents/CYRS/CYRS_Review.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\software\project\Input documents\CYRS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction " sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction " sheetId="1" r:id="rId1"/>
+    <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">#REF!</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,12 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
   <si>
-    <t xml:space="preserve">Electric Blender</t>
+    <t>Electric Blender</t>
   </si>
   <si>
     <t xml:space="preserve">Ref Document </t>
@@ -41,25 +45,25 @@
     <t xml:space="preserve">Ref Version </t>
   </si>
   <si>
-    <t xml:space="preserve">V2.1</t>
+    <t>V2.1</t>
   </si>
   <si>
     <t xml:space="preserve">Auther </t>
   </si>
   <si>
-    <t xml:space="preserve">Abdelrahman Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auther</t>
+    <t>Abdelrahman Ali</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Auther</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -68,85 +72,85 @@
     <t xml:space="preserve">Change </t>
   </si>
   <si>
-    <t xml:space="preserve">A.Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2020</t>
+    <t>A.Ali</t>
+  </si>
+  <si>
+    <t>29/01/2020</t>
   </si>
   <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Update review sheet &amp; close old points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entry Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page/Line/Section/Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open point : description of problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V0.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 1</t>
+    <t>Update review sheet &amp; close old points</t>
+  </si>
+  <si>
+    <t>Entry Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Detection version</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>Page/Line/Section/Entity</t>
+  </si>
+  <si>
+    <t>Open point : description of problem</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>V0.2</t>
+  </si>
+  <si>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>Page 1</t>
   </si>
   <si>
     <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Releases after accomplishing cross review on it. </t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All pages</t>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>All pages</t>
   </si>
   <si>
     <t xml:space="preserve">Redundancy in Version field besides Date in header table. </t>
   </si>
   <si>
-    <t xml:space="preserve">Contents</t>
+    <t>Contents</t>
   </si>
   <si>
     <t xml:space="preserve">Update Table of Content numbering specially for Functional Requirements section. </t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
+    <t>All</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even CYRS should have one and the reference is the customer Requirement for the product </t>
   </si>
   <si>
-    <t xml:space="preserve">Refused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Requirements</t>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>Functional Requirements</t>
   </si>
   <si>
     <t xml:space="preserve">You need to make your requirement more clarified from the system level prospective. 
@@ -165,7 +169,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">REQ_PO2EBL_CYRS_03_V02 :</t>
+      <t>REQ_PO2EBL_CYRS_03_V02 :</t>
     </r>
     <r>
       <rPr>
@@ -188,7 +192,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Open</t>
+    <t>Open</t>
   </si>
   <si>
     <t xml:space="preserve">REQ_PO2EBL_CYRS_04_V02: 
@@ -196,25 +200,25 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">V1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version Date is different from the Date field in Release Table in page 2 , please apply a unique Date format for all date fields, add a title before the table in second page.</t>
+    <t>V1.8</t>
+  </si>
+  <si>
+    <t>Version Date is different from the Date field in Release Table in page 2 , please apply a unique Date format for all date fields, add a title before the table in second page.</t>
   </si>
   <si>
     <t xml:space="preserve">AAL 10/2/2020 : there’s no title added before the table in second page. </t>
   </si>
   <si>
-    <t xml:space="preserve">Page 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As discussed before Hardware Section shall be written in HSI document and instead of this section you can add a block diagram which describe how the system components interact with each others (I/Ps &amp; O/Ps).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAL 10/2/2020: add a block diagram which describe how the system components interact with each others (I/Ps &amp; O/Ps).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 3</t>
+    <t>Page 6</t>
+  </si>
+  <si>
+    <t>As discussed before Hardware Section shall be written in HSI document and instead of this section you can add a block diagram which describe how the system components interact with each others (I/Ps &amp; O/Ps).</t>
+  </si>
+  <si>
+    <t>AAL 10/2/2020: add a block diagram which describe how the system components interact with each others (I/Ps &amp; O/Ps).</t>
+  </si>
+  <si>
+    <t>Page 3</t>
   </si>
   <si>
     <t xml:space="preserve">In Revision table, the description column shall include the requirement IDs (modified/added or deleted) from CYRS document and a small description or brief about what changed in this requirement.  </t>
@@ -226,10 +230,10 @@
     <t xml:space="preserve">whether to accept the open point if you see applicable and valid or to refuse it and give a justification in the comment field whether you accept , then update with the action you did , or refuse with justification </t>
   </si>
   <si>
-    <t xml:space="preserve">System Requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You need to add more requirements in CYRS which illustrate some features in your system 
+    <t>System Requirements</t>
+  </si>
+  <si>
+    <t>You need to add more requirements in CYRS which illustrate some features in your system 
 Ex: you can  add requirements which describe how to handle the communication between the inputs devices &amp; o/p devices.</t>
   </si>
   <si>
@@ -242,17 +246,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]General"/>
-    <numFmt numFmtId="168" formatCode="[$-409]M/D/YYYY"/>
-    <numFmt numFmtId="169" formatCode="@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]MM/DD/YY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]General"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
+    <numFmt numFmtId="168" formatCode="[$-409]mm/dd/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -261,22 +263,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -290,7 +277,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -312,6 +299,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -345,103 +339,149 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -457,214 +497,161 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 3 2" xfId="20"/>
-    <cellStyle name="Normal 4" xfId="21"/>
-    <cellStyle name="Excel Built-in Accent3" xfId="22"/>
+    <cellStyle name="Normal 3 2" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
     <dxf>
       <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
         <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
       </font>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -723,238 +710,516 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.27"/>
+    <col min="8" max="8" width="32.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4" t="n">
+      <c r="C9" s="13"/>
+      <c r="D9" s="10">
         <v>44106</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="15">
         <v>0.1</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="5"/>
+      <c r="G13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="n">
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="15">
         <v>0.2</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12" t="n">
+      <c r="D14" s="5"/>
+      <c r="E14" s="4">
         <v>44014</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="n">
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="15">
         <v>0.3</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12" t="n">
+      <c r="D15" s="5"/>
+      <c r="E15" s="4">
         <v>44106</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="15"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="15"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="16"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -962,57 +1227,45 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="100.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="9" max="9" width="32.90625" customWidth="1"/>
+    <col min="12" max="12" width="174.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
@@ -1041,7 +1294,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>15</v>
       </c>
@@ -1068,7 +1321,7 @@
       </c>
       <c r="I2" s="25"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1095,7 +1348,7 @@
       </c>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
@@ -1121,11 +1374,11 @@
         <v>32</v>
       </c>
       <c r="I4" s="25"/>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>15</v>
       </c>
@@ -1151,11 +1404,11 @@
         <v>32</v>
       </c>
       <c r="I5" s="25"/>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1184,7 +1437,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="52.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" ht="52.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
@@ -1210,11 +1463,11 @@
         <v>32</v>
       </c>
       <c r="I7" s="25"/>
-      <c r="K7" s="0" t="s">
+      <c r="K7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
@@ -1240,12 +1493,12 @@
         <v>32</v>
       </c>
       <c r="I8" s="23"/>
-      <c r="K8" s="0" t="s">
+      <c r="K8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="n">
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="27">
         <v>44014</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -1263,7 +1516,9 @@
       <c r="F9" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="25"/>
+      <c r="G9" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="25" t="s">
         <v>44</v>
       </c>
@@ -1271,8 +1526,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="n">
+    <row r="10" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="27">
         <v>44014</v>
       </c>
       <c r="B10" s="21" t="s">
@@ -1290,7 +1545,9 @@
       <c r="F10" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="H10" s="25" t="s">
         <v>44</v>
       </c>
@@ -1298,8 +1555,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="n">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="27">
         <v>44014</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -1317,20 +1574,22 @@
       <c r="F11" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="H11" s="25" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="23"/>
-      <c r="K11" s="0" t="s">
+      <c r="K11" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="L11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="n">
+    <row r="12" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="27">
         <v>44106</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -1348,19 +1607,21 @@
       <c r="F12" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="H12" s="25" t="s">
         <v>44</v>
       </c>
       <c r="I12" s="23"/>
-      <c r="K12" s="0" t="s">
+      <c r="K12" t="s">
         <v>58</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="L12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -1371,7 +1632,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="23"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="27"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -1382,7 +1643,7 @@
       <c r="H14" s="25"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="27"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -1393,7 +1654,7 @@
       <c r="H15" s="25"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -1404,7 +1665,7 @@
       <c r="H16" s="25"/>
       <c r="I16" s="33"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="28"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -1415,7 +1676,7 @@
       <c r="H17" s="25"/>
       <c r="I17" s="33"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
@@ -1426,7 +1687,7 @@
       <c r="H18" s="25"/>
       <c r="I18" s="33"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="30"/>
@@ -1437,7 +1698,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="33"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="30"/>
@@ -1448,7 +1709,7 @@
       <c r="H20" s="25"/>
       <c r="I20" s="33"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
       <c r="C21" s="30"/>
@@ -1459,7 +1720,7 @@
       <c r="H21" s="25"/>
       <c r="I21" s="33"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="30"/>
@@ -1470,7 +1731,7 @@
       <c r="H22" s="25"/>
       <c r="I22" s="33"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="30"/>
@@ -1481,7 +1742,7 @@
       <c r="H23" s="25"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="30"/>
@@ -1492,7 +1753,7 @@
       <c r="H24" s="25"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="30"/>
@@ -1503,7 +1764,7 @@
       <c r="H25" s="25"/>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="28"/>
       <c r="B26" s="29"/>
       <c r="C26" s="30"/>
@@ -1514,7 +1775,7 @@
       <c r="H26" s="25"/>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="28"/>
       <c r="B27" s="29"/>
       <c r="C27" s="30"/>
@@ -1525,7 +1786,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="30"/>
       <c r="B28" s="30"/>
       <c r="C28" s="30"/>
@@ -1536,7 +1797,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="28"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -1547,7 +1808,7 @@
       <c r="H29" s="25"/>
       <c r="I29" s="33"/>
     </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="28"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -1558,7 +1819,7 @@
       <c r="H30" s="25"/>
       <c r="I30" s="33"/>
     </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="28"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -1569,7 +1830,7 @@
       <c r="H31" s="25"/>
       <c r="I31" s="33"/>
     </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="30"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -1580,7 +1841,7 @@
       <c r="H32" s="25"/>
       <c r="I32" s="33"/>
     </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -1591,7 +1852,7 @@
       <c r="H33" s="25"/>
       <c r="I33" s="33"/>
     </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
@@ -1602,7 +1863,7 @@
       <c r="H34" s="25"/>
       <c r="I34" s="33"/>
     </row>
-    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -1613,7 +1874,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="33"/>
     </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="30"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -1624,7 +1885,7 @@
       <c r="H36" s="25"/>
       <c r="I36" s="33"/>
     </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -1635,7 +1896,7 @@
       <c r="H37" s="25"/>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -1646,7 +1907,7 @@
       <c r="H38" s="25"/>
       <c r="I38" s="33"/>
     </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -1657,7 +1918,7 @@
       <c r="H39" s="25"/>
       <c r="I39" s="33"/>
     </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -1668,7 +1929,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -1679,7 +1940,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -1690,7 +1951,7 @@
       <c r="H42" s="25"/>
       <c r="I42" s="33"/>
     </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="30"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
@@ -1701,7 +1962,7 @@
       <c r="H43" s="25"/>
       <c r="I43" s="33"/>
     </row>
-    <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="30"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
@@ -1712,7 +1973,7 @@
       <c r="H44" s="25"/>
       <c r="I44" s="33"/>
     </row>
-    <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="30"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
@@ -1723,7 +1984,7 @@
       <c r="H45" s="25"/>
       <c r="I45" s="33"/>
     </row>
-    <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="30"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
@@ -1734,7 +1995,7 @@
       <c r="H46" s="25"/>
       <c r="I46" s="33"/>
     </row>
-    <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="30"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -1747,44 +2008,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1047" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1047">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1 H23:H1047" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1 H23:H1047">
       <formula1>$K$8:$K$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H22" type="list">
-      <formula1>'Cross review points '!$K$7:$K$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H22">
+      <formula1>$K$7:$K$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>